<commit_message>
updated data from quant engine
</commit_message>
<xml_diff>
--- a/mf-intelligence/data/processed/quant/quant_Aggressive_Hybrid_Fund_Equity_Holdings_Comparison.xlsx
+++ b/mf-intelligence/data/processed/quant/quant_Aggressive_Hybrid_Fund_Equity_Holdings_Comparison.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,17 +451,17 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>Jan_2026</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>Dec_2025</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Nov_2025</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Oct_2025</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
@@ -478,12 +478,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>INE018A01030</t>
+          <t>INE040A01034</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Larsen &amp; Toubro Limited</t>
+          <t>HDFC Bank Limited</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -492,30 +492,30 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>7.795835</v>
+        <v>8.303181</v>
       </c>
       <c r="E2" t="n">
-        <v>7.650868</v>
+        <v>0.486552</v>
       </c>
       <c r="F2" t="n">
-        <v>7.511396</v>
+        <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>0.1449670000000003</v>
+        <v>7.816629000000001</v>
       </c>
       <c r="H2" t="n">
-        <v>0.2844389999999999</v>
+        <v>8.303181</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>INE758E01017</t>
+          <t>INE018A01030</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Jio Financial Services Limited</t>
+          <t>Larsen &amp; Toubro Limited</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -524,19 +524,19 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>7.429747</v>
+        <v>7.967097</v>
       </c>
       <c r="E3" t="n">
-        <v>7.595557</v>
+        <v>7.795835</v>
       </c>
       <c r="F3" t="n">
-        <v>7.543441</v>
+        <v>7.650868</v>
       </c>
       <c r="G3" t="n">
-        <v>-0.1658100000000005</v>
+        <v>0.1712619999999996</v>
       </c>
       <c r="H3" t="n">
-        <v>-0.1136939999999997</v>
+        <v>0.3162289999999999</v>
       </c>
     </row>
     <row r="4">
@@ -556,30 +556,30 @@
         </is>
       </c>
       <c r="D4" t="n">
+        <v>7.270346</v>
+      </c>
+      <c r="E4" t="n">
         <v>7.235738</v>
       </c>
-      <c r="E4" t="n">
+      <c r="F4" t="n">
         <v>7.349683</v>
       </c>
-      <c r="F4" t="n">
-        <v>7.796691</v>
-      </c>
       <c r="G4" t="n">
-        <v>-0.1139450000000002</v>
+        <v>0.03460800000000042</v>
       </c>
       <c r="H4" t="n">
-        <v>-0.5609530000000005</v>
+        <v>-0.07933699999999977</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>INE364U01010</t>
+          <t>INE917I01010</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Adani Green Energy Limited</t>
+          <t>Bajaj Auto Limited</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -588,30 +588,30 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>6.64915</v>
+        <v>7.01815</v>
       </c>
       <c r="E5" t="n">
-        <v>3.708483</v>
+        <v>6.437652</v>
       </c>
       <c r="F5" t="n">
-        <v>3.99776</v>
+        <v>5.181581</v>
       </c>
       <c r="G5" t="n">
-        <v>2.940666999999999</v>
+        <v>0.5804980000000004</v>
       </c>
       <c r="H5" t="n">
-        <v>2.65139</v>
+        <v>1.836569</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>INE917I01010</t>
+          <t>INE090A01021</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Bajaj Auto Limited</t>
+          <t>ICICI Bank Limited</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -620,30 +620,30 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>6.437652</v>
+        <v>6.16377</v>
       </c>
       <c r="E6" t="n">
-        <v>5.181581</v>
+        <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>5.03351</v>
+        <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>1.256070999999999</v>
+        <v>6.16377</v>
       </c>
       <c r="H6" t="n">
-        <v>1.404142</v>
+        <v>6.16377</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>INE216A01030</t>
+          <t>INE364U01010</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Britannia Industries Limited</t>
+          <t>Adani Green Energy Limited</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -652,19 +652,19 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>6.408499</v>
+        <v>5.924793</v>
       </c>
       <c r="E7" t="n">
-        <v>6.117228</v>
+        <v>6.64915</v>
       </c>
       <c r="F7" t="n">
-        <v>6.05352</v>
+        <v>3.708483</v>
       </c>
       <c r="G7" t="n">
-        <v>0.2912710000000001</v>
+        <v>-0.7243569999999995</v>
       </c>
       <c r="H7" t="n">
-        <v>0.3549790000000002</v>
+        <v>2.21631</v>
       </c>
     </row>
     <row r="8">
@@ -684,30 +684,30 @@
         </is>
       </c>
       <c r="D8" t="n">
+        <v>5.775625</v>
+      </c>
+      <c r="E8" t="n">
         <v>5.58255</v>
       </c>
-      <c r="E8" t="n">
+      <c r="F8" t="n">
         <v>5.603391</v>
       </c>
-      <c r="F8" t="n">
-        <v>5.318251</v>
-      </c>
       <c r="G8" t="n">
-        <v>-0.02084099999999989</v>
+        <v>0.1930749999999994</v>
       </c>
       <c r="H8" t="n">
-        <v>0.2642990000000003</v>
+        <v>0.1722339999999996</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>INE002A01018</t>
+          <t>INE556F16BR2</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Reliance Industries Limited</t>
+          <t>SIDBI CD 10-Nov-2026</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -716,19 +716,19 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>5.255267</v>
+        <v>4.834687</v>
       </c>
       <c r="E9" t="n">
-        <v>8.443042</v>
+        <v>4.551729</v>
       </c>
       <c r="F9" t="n">
-        <v>7.935728</v>
+        <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>-3.187775</v>
+        <v>0.2829579999999998</v>
       </c>
       <c r="H9" t="n">
-        <v>-2.680461</v>
+        <v>4.834687</v>
       </c>
     </row>
     <row r="10">
@@ -748,30 +748,30 @@
         </is>
       </c>
       <c r="D10" t="n">
+        <v>4.516326</v>
+      </c>
+      <c r="E10" t="n">
         <v>4.717528</v>
       </c>
-      <c r="E10" t="n">
+      <c r="F10" t="n">
         <v>3.448005</v>
       </c>
-      <c r="F10" t="n">
-        <v>3.718617</v>
-      </c>
       <c r="G10" t="n">
-        <v>1.269523</v>
+        <v>-0.2012019999999994</v>
       </c>
       <c r="H10" t="n">
-        <v>0.9989109999999997</v>
+        <v>1.068321</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>INE556F16BR2</t>
+          <t>INE775A01035</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>SIDBI CD 10-Nov-2026</t>
+          <t>Samvardhana Motherson International Ltd</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -780,30 +780,30 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>4.551729</v>
+        <v>3.673839</v>
       </c>
       <c r="E11" t="n">
-        <v>0</v>
+        <v>3.67762</v>
       </c>
       <c r="F11" t="n">
         <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>4.551729</v>
+        <v>-0.003781000000000034</v>
       </c>
       <c r="H11" t="n">
-        <v>4.551729</v>
+        <v>3.673839</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>INE245A01021</t>
+          <t>INE406A01037</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Tata Power Company Limited</t>
+          <t>Aurobindo Pharma Limited</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -812,30 +812,30 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>3.840354</v>
+        <v>3.444555</v>
       </c>
       <c r="E12" t="n">
-        <v>5.288741</v>
+        <v>3.13663</v>
       </c>
       <c r="F12" t="n">
-        <v>5.441064</v>
+        <v>3.202917</v>
       </c>
       <c r="G12" t="n">
-        <v>-1.448387</v>
+        <v>0.307925</v>
       </c>
       <c r="H12" t="n">
-        <v>-1.60071</v>
+        <v>0.241638</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>INE775A01035</t>
+          <t>INE758E01017</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Samvardhana Motherson International Ltd</t>
+          <t>Jio Financial Services Limited</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -844,30 +844,30 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>3.67762</v>
+        <v>3.106554</v>
       </c>
       <c r="E13" t="n">
-        <v>0</v>
+        <v>7.429747</v>
       </c>
       <c r="F13" t="n">
-        <v>0</v>
+        <v>7.595557</v>
       </c>
       <c r="G13" t="n">
-        <v>3.67762</v>
+        <v>-4.323193</v>
       </c>
       <c r="H13" t="n">
-        <v>3.67762</v>
+        <v>-4.489003</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>INE406A01037</t>
+          <t>INE127D01025</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Aurobindo Pharma Limited</t>
+          <t>HDFC Asset Management Company Ltd</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -876,19 +876,19 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>3.13663</v>
+        <v>2.975697</v>
       </c>
       <c r="E14" t="n">
-        <v>3.202917</v>
+        <v>0</v>
       </c>
       <c r="F14" t="n">
-        <v>2.947492</v>
+        <v>0</v>
       </c>
       <c r="G14" t="n">
-        <v>-0.06628699999999998</v>
+        <v>2.975697</v>
       </c>
       <c r="H14" t="n">
-        <v>0.1891379999999998</v>
+        <v>2.975697</v>
       </c>
     </row>
     <row r="15">
@@ -908,30 +908,30 @@
         </is>
       </c>
       <c r="D15" t="n">
+        <v>1.895889</v>
+      </c>
+      <c r="E15" t="n">
         <v>1.810264</v>
       </c>
-      <c r="E15" t="n">
+      <c r="F15" t="n">
         <v>1.825513</v>
       </c>
-      <c r="F15" t="n">
-        <v>1.814661</v>
-      </c>
       <c r="G15" t="n">
-        <v>-0.01524899999999985</v>
+        <v>0.08562499999999984</v>
       </c>
       <c r="H15" t="n">
-        <v>-0.004396999999999984</v>
+        <v>0.07037599999999999</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>INE040A01034</t>
+          <t>INE721A01047</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>HDFC Bank Limited</t>
+          <t>Shriram Finance Limited</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -940,7 +940,7 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>0.486552</v>
+        <v>1.450518</v>
       </c>
       <c r="E16" t="n">
         <v>0</v>
@@ -949,21 +949,21 @@
         <v>0</v>
       </c>
       <c r="G16" t="n">
-        <v>0.486552</v>
+        <v>1.450518</v>
       </c>
       <c r="H16" t="n">
-        <v>0.486552</v>
+        <v>1.450518</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>INE669C01036</t>
+          <t>INE245A01021</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Tech Mahindra Limited</t>
+          <t>Tata Power Company Limited</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -972,30 +972,30 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>0.335577</v>
+        <v>0</v>
       </c>
       <c r="E17" t="n">
-        <v>0</v>
+        <v>3.840354</v>
       </c>
       <c r="F17" t="n">
-        <v>0</v>
+        <v>5.288741</v>
       </c>
       <c r="G17" t="n">
-        <v>0.335577</v>
+        <v>-3.840354</v>
       </c>
       <c r="H17" t="n">
-        <v>0.335577</v>
+        <v>-5.288741</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>INE202B01038</t>
+          <t>INE423A20016</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Piramal Finance Ltd</t>
+          <t>Adani Enterprises Limited Rights</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1010,24 +1010,24 @@
         <v>0</v>
       </c>
       <c r="F18" t="n">
-        <v>0.114857</v>
+        <v>0.080276</v>
       </c>
       <c r="G18" t="n">
         <v>0</v>
       </c>
       <c r="H18" t="n">
-        <v>-0.114857</v>
+        <v>-0.080276</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>INE423A20016</t>
+          <t>INE216A01030</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Adani Enterprises Limited Rights</t>
+          <t>Britannia Industries Limited</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1039,27 +1039,27 @@
         <v>0</v>
       </c>
       <c r="E19" t="n">
-        <v>0.080276</v>
+        <v>6.408499</v>
       </c>
       <c r="F19" t="n">
-        <v>0</v>
+        <v>6.117228</v>
       </c>
       <c r="G19" t="n">
-        <v>-0.080276</v>
+        <v>-6.408499</v>
       </c>
       <c r="H19" t="n">
-        <v>0</v>
+        <v>-6.117228</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>INE0J1Y01017</t>
+          <t>INE669C01036</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Life Insurance Corporation Of India</t>
+          <t>Tech Mahindra Limited</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1071,16 +1071,16 @@
         <v>0</v>
       </c>
       <c r="E20" t="n">
-        <v>0</v>
+        <v>0.335577</v>
       </c>
       <c r="F20" t="n">
-        <v>6.257899</v>
+        <v>0</v>
       </c>
       <c r="G20" t="n">
-        <v>0</v>
+        <v>-0.335577</v>
       </c>
       <c r="H20" t="n">
-        <v>-6.257899</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -1103,16 +1103,48 @@
         <v>0</v>
       </c>
       <c r="E21" t="n">
+        <v>0</v>
+      </c>
+      <c r="F21" t="n">
         <v>5.281295</v>
       </c>
-      <c r="F21" t="n">
-        <v>5.010222</v>
-      </c>
       <c r="G21" t="n">
+        <v>0</v>
+      </c>
+      <c r="H21" t="n">
         <v>-5.281295</v>
       </c>
-      <c r="H21" t="n">
-        <v>-5.010222</v>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>INE002A01018</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Reliance Industries Limited</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>quant Aggressive Hybrid Fund</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>0</v>
+      </c>
+      <c r="E22" t="n">
+        <v>5.255267</v>
+      </c>
+      <c r="F22" t="n">
+        <v>8.443042</v>
+      </c>
+      <c r="G22" t="n">
+        <v>-5.255267</v>
+      </c>
+      <c r="H22" t="n">
+        <v>-8.443042</v>
       </c>
     </row>
   </sheetData>

</xml_diff>